<commit_message>
Into BA: added the exercises
</commit_message>
<xml_diff>
--- a/Introduction_to_Business_Analytics/Examples/Lecture 4 - Forecasting Techniques in Excel.xlsx
+++ b/Introduction_to_Business_Analytics/Examples/Lecture 4 - Forecasting Techniques in Excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://abofi-my.sharepoint.com/personal/xiaolu_wang_abo_fi/Documents/Teaching/Introduction to Business Analytics/Introduction to Business Analytics (2024-2025)/Lecture 4 - Forecasting Techniques in Excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hektor\Desktop\Kurser\2024-2025\Uni_2024_2025\Introduction_to_Business_Analytics\Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="377" documentId="13_ncr:1_{42DE5E25-6DDF-4009-87A0-3A0AE084E038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FDAA838A-4F44-6C49-B96B-CEB464F00569}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AE84E63-CB75-4D17-8953-F4AEBE395E67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
@@ -2048,7 +2048,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="39">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -2380,32 +2380,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
@@ -2449,17 +2423,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color auto="1"/>
       </left>
@@ -2485,17 +2448,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2510,7 +2462,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
@@ -2797,34 +2749,81 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="2" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="2" fontId="8" fillId="5" borderId="33" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="8" fillId="5" borderId="31" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="2" fontId="10" fillId="3" borderId="33" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="10" fillId="3" borderId="31" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="10" fontId="11" fillId="2" borderId="32" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="10" fontId="11" fillId="2" borderId="30" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="2" fontId="8" fillId="6" borderId="34" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="8" fillId="6" borderId="32" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="10" fontId="11" fillId="2" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="25" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="16" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2835,19 +2834,11 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="25" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="16" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="36" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="37" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -2855,73 +2846,7 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="35" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="31" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="11" fillId="2" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="10" fillId="3" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -2933,7 +2858,7 @@
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Per cent" xfId="6" builtinId="5"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
     <cellStyle name="Style 1" xfId="7" xr:uid="{484D713F-AD31-6F4B-B7BC-C092C53F7B53}"/>
   </cellStyles>
   <dxfs count="2">
@@ -3316,10 +3241,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3607,37 +3528,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A21:AJ71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" topLeftCell="G24" zoomScale="105" zoomScaleNormal="160" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="I70" sqref="I70:J70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="1" width="8.6640625" style="2"/>
-    <col min="2" max="2" width="18.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" style="2" customWidth="1"/>
     <col min="6" max="6" width="13" style="2" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12.5" style="2" customWidth="1"/>
-    <col min="9" max="9" width="9.83203125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="19.1640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.77734375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="9.77734375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="19.109375" style="2" customWidth="1"/>
     <col min="11" max="12" width="12.6640625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="12.1640625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="12.109375" style="2" customWidth="1"/>
     <col min="14" max="14" width="12.33203125" style="2" customWidth="1"/>
-    <col min="15" max="15" width="10.5" style="2" customWidth="1"/>
+    <col min="15" max="15" width="10.44140625" style="2" customWidth="1"/>
     <col min="16" max="16" width="19.6640625" style="3" customWidth="1"/>
     <col min="17" max="17" width="12.6640625" style="2" customWidth="1"/>
     <col min="18" max="18" width="12" style="2" customWidth="1"/>
-    <col min="19" max="19" width="11.83203125" style="2" customWidth="1"/>
-    <col min="20" max="20" width="13.5" style="3" customWidth="1"/>
-    <col min="21" max="21" width="10.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.77734375" style="2" customWidth="1"/>
+    <col min="20" max="20" width="13.44140625" style="3" customWidth="1"/>
+    <col min="21" max="21" width="10.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="23" max="16384" width="8.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="21" spans="1:36" ht="14" thickBot="1">
+    <row r="21" spans="1:36" ht="13.8" thickBot="1">
       <c r="A21" s="1" t="s">
         <v>1</v>
       </c>
@@ -3680,7 +3601,7 @@
       <c r="AI22" s="9"/>
       <c r="AJ22" s="9"/>
     </row>
-    <row r="23" spans="1:36" ht="15">
+    <row r="23" spans="1:36" ht="14.4">
       <c r="C23" s="10" t="s">
         <v>5</v>
       </c>
@@ -3721,7 +3642,7 @@
       <c r="AI23" s="9"/>
       <c r="AJ23" s="9"/>
     </row>
-    <row r="24" spans="1:36" ht="33" thickBot="1">
+    <row r="24" spans="1:36" ht="29.4" thickBot="1">
       <c r="A24" s="17" t="s">
         <v>0</v>
       </c>
@@ -3798,7 +3719,7 @@
       <c r="AI24" s="9"/>
       <c r="AJ24" s="9"/>
     </row>
-    <row r="25" spans="1:36" s="20" customFormat="1" ht="16" thickTop="1">
+    <row r="25" spans="1:36" s="20" customFormat="1" ht="15" thickTop="1">
       <c r="A25" s="20">
         <v>1</v>
       </c>
@@ -3836,7 +3757,7 @@
       <c r="AI25" s="42"/>
       <c r="AJ25" s="42"/>
     </row>
-    <row r="26" spans="1:36" s="20" customFormat="1" ht="15">
+    <row r="26" spans="1:36" s="20" customFormat="1" ht="14.4">
       <c r="A26" s="20">
         <v>2</v>
       </c>
@@ -3876,19 +3797,37 @@
       <c r="AI26" s="42"/>
       <c r="AJ26" s="42"/>
     </row>
-    <row r="27" spans="1:36" s="20" customFormat="1" ht="15">
+    <row r="27" spans="1:36" s="20" customFormat="1" ht="14.4">
       <c r="A27" s="20">
         <v>3</v>
       </c>
       <c r="B27" s="20">
         <v>60</v>
       </c>
-      <c r="C27" s="22"/>
-      <c r="D27" s="77"/>
-      <c r="E27" s="44"/>
-      <c r="F27" s="61"/>
-      <c r="G27" s="62"/>
-      <c r="H27" s="75"/>
+      <c r="C27" s="22">
+        <f>AVERAGE(B25:B26)</f>
+        <v>66</v>
+      </c>
+      <c r="D27" s="76">
+        <f>AVERAGE(B25:B26)</f>
+        <v>66</v>
+      </c>
+      <c r="E27" s="44">
+        <f>B27-C27</f>
+        <v>-6</v>
+      </c>
+      <c r="F27" s="61">
+        <f>ABS(E27)</f>
+        <v>6</v>
+      </c>
+      <c r="G27" s="62">
+        <f>E27^2</f>
+        <v>36</v>
+      </c>
+      <c r="H27" s="75">
+        <f>F27/B27</f>
+        <v>0.1</v>
+      </c>
       <c r="J27"/>
       <c r="K27" s="43"/>
       <c r="L27" s="63"/>
@@ -3916,25 +3855,61 @@
       <c r="AI27" s="42"/>
       <c r="AJ27" s="42"/>
     </row>
-    <row r="28" spans="1:36" s="20" customFormat="1" ht="15">
+    <row r="28" spans="1:36" s="20" customFormat="1" ht="14.4">
       <c r="A28" s="20">
         <v>4</v>
       </c>
       <c r="B28" s="20">
         <v>56</v>
       </c>
-      <c r="C28" s="22"/>
-      <c r="D28" s="77"/>
-      <c r="E28" s="44"/>
-      <c r="F28" s="61"/>
-      <c r="G28" s="62"/>
-      <c r="H28" s="75"/>
-      <c r="I28" s="31"/>
-      <c r="J28" s="77"/>
-      <c r="K28" s="44"/>
-      <c r="L28" s="61"/>
-      <c r="M28" s="62"/>
-      <c r="N28" s="75"/>
+      <c r="C28" s="22">
+        <f t="shared" ref="C28:C41" si="0">AVERAGE(B26:B27)</f>
+        <v>52</v>
+      </c>
+      <c r="D28" s="76">
+        <f t="shared" ref="D28:D42" si="1">AVERAGE(B26:B27)</f>
+        <v>52</v>
+      </c>
+      <c r="E28" s="44">
+        <f t="shared" ref="E28:E42" si="2">B28-C28</f>
+        <v>4</v>
+      </c>
+      <c r="F28" s="61">
+        <f t="shared" ref="F28:F42" si="3">ABS(E28)</f>
+        <v>4</v>
+      </c>
+      <c r="G28" s="62">
+        <f t="shared" ref="G28:G41" si="4">E28^2</f>
+        <v>16</v>
+      </c>
+      <c r="H28" s="75">
+        <f t="shared" ref="H28:H41" si="5">F28/B28</f>
+        <v>7.1428571428571425E-2</v>
+      </c>
+      <c r="I28" s="31">
+        <f>AVERAGE(B25:B27)</f>
+        <v>64</v>
+      </c>
+      <c r="J28" s="76">
+        <f>AVERAGE(B25:B27)</f>
+        <v>64</v>
+      </c>
+      <c r="K28" s="44">
+        <f>B28-I28</f>
+        <v>-8</v>
+      </c>
+      <c r="L28" s="61">
+        <f>ABS(K28)</f>
+        <v>8</v>
+      </c>
+      <c r="M28" s="62">
+        <f>K28^2</f>
+        <v>64</v>
+      </c>
+      <c r="N28" s="75">
+        <f>L28/B28</f>
+        <v>0.14285714285714285</v>
+      </c>
       <c r="O28" s="21"/>
       <c r="P28"/>
       <c r="Q28" s="37"/>
@@ -3957,31 +3932,85 @@
       <c r="AI28" s="42"/>
       <c r="AJ28" s="42"/>
     </row>
-    <row r="29" spans="1:36" s="20" customFormat="1" ht="15">
+    <row r="29" spans="1:36" s="20" customFormat="1" ht="14.4">
       <c r="A29" s="20">
         <v>5</v>
       </c>
       <c r="B29" s="20">
         <v>70</v>
       </c>
-      <c r="C29" s="22"/>
-      <c r="D29" s="77"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="61"/>
-      <c r="G29" s="62"/>
-      <c r="H29" s="75"/>
-      <c r="I29" s="31"/>
-      <c r="J29" s="77"/>
-      <c r="K29" s="44"/>
-      <c r="L29" s="61"/>
-      <c r="M29" s="62"/>
-      <c r="N29" s="75"/>
-      <c r="O29" s="22"/>
-      <c r="P29" s="77"/>
-      <c r="Q29" s="44"/>
-      <c r="R29" s="66"/>
-      <c r="S29" s="62"/>
-      <c r="T29" s="75"/>
+      <c r="C29" s="22">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="D29" s="76">
+        <f t="shared" si="1"/>
+        <v>58</v>
+      </c>
+      <c r="E29" s="44">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="F29" s="61">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="G29" s="62">
+        <f t="shared" si="4"/>
+        <v>144</v>
+      </c>
+      <c r="H29" s="75">
+        <f t="shared" si="5"/>
+        <v>0.17142857142857143</v>
+      </c>
+      <c r="I29" s="31">
+        <f t="shared" ref="I29:I41" si="6">AVERAGE(B26:B28)</f>
+        <v>53.333333333333336</v>
+      </c>
+      <c r="J29" s="76">
+        <f t="shared" ref="J29:J42" si="7">AVERAGE(B26:B28)</f>
+        <v>53.333333333333336</v>
+      </c>
+      <c r="K29" s="44">
+        <f t="shared" ref="K29:K41" si="8">B29-I29</f>
+        <v>16.666666666666664</v>
+      </c>
+      <c r="L29" s="61">
+        <f t="shared" ref="L29:L41" si="9">ABS(K29)</f>
+        <v>16.666666666666664</v>
+      </c>
+      <c r="M29" s="62">
+        <f t="shared" ref="M29:M41" si="10">K29^2</f>
+        <v>277.77777777777771</v>
+      </c>
+      <c r="N29" s="75">
+        <f t="shared" ref="N29:N41" si="11">L29/B29</f>
+        <v>0.23809523809523805</v>
+      </c>
+      <c r="O29" s="22">
+        <f>AVERAGE(B25:B28)</f>
+        <v>62</v>
+      </c>
+      <c r="P29" s="76">
+        <f>AVERAGE(B25:B28)</f>
+        <v>62</v>
+      </c>
+      <c r="Q29" s="44">
+        <f>B29-O29</f>
+        <v>8</v>
+      </c>
+      <c r="R29" s="66">
+        <f>ABS(Q29)</f>
+        <v>8</v>
+      </c>
+      <c r="S29" s="62">
+        <f>Q29^2</f>
+        <v>64</v>
+      </c>
+      <c r="T29" s="75">
+        <f>R29/ABS(B29)</f>
+        <v>0.11428571428571428</v>
+      </c>
       <c r="V29" s="42"/>
       <c r="W29" s="42"/>
       <c r="X29" s="42"/>
@@ -3998,31 +4027,85 @@
       <c r="AI29" s="42"/>
       <c r="AJ29" s="42"/>
     </row>
-    <row r="30" spans="1:36" s="20" customFormat="1" ht="15">
+    <row r="30" spans="1:36" s="20" customFormat="1" ht="14.4">
       <c r="A30" s="20">
         <v>6</v>
       </c>
       <c r="B30" s="20">
         <v>91</v>
       </c>
-      <c r="C30" s="22"/>
-      <c r="D30" s="77"/>
-      <c r="E30" s="44"/>
-      <c r="F30" s="61"/>
-      <c r="G30" s="62"/>
-      <c r="H30" s="75"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="77"/>
-      <c r="K30" s="44"/>
-      <c r="L30" s="61"/>
-      <c r="M30" s="62"/>
-      <c r="N30" s="75"/>
-      <c r="O30" s="22"/>
-      <c r="P30" s="77"/>
-      <c r="Q30" s="44"/>
-      <c r="R30" s="66"/>
-      <c r="S30" s="62"/>
-      <c r="T30" s="75"/>
+      <c r="C30" s="22">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="D30" s="76">
+        <f t="shared" si="1"/>
+        <v>63</v>
+      </c>
+      <c r="E30" s="44">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="F30" s="61">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+      <c r="G30" s="62">
+        <f t="shared" si="4"/>
+        <v>784</v>
+      </c>
+      <c r="H30" s="75">
+        <f t="shared" si="5"/>
+        <v>0.30769230769230771</v>
+      </c>
+      <c r="I30" s="31">
+        <f t="shared" si="6"/>
+        <v>62</v>
+      </c>
+      <c r="J30" s="76">
+        <f t="shared" si="7"/>
+        <v>62</v>
+      </c>
+      <c r="K30" s="44">
+        <f t="shared" si="8"/>
+        <v>29</v>
+      </c>
+      <c r="L30" s="61">
+        <f t="shared" si="9"/>
+        <v>29</v>
+      </c>
+      <c r="M30" s="62">
+        <f t="shared" si="10"/>
+        <v>841</v>
+      </c>
+      <c r="N30" s="75">
+        <f t="shared" si="11"/>
+        <v>0.31868131868131866</v>
+      </c>
+      <c r="O30" s="22">
+        <f t="shared" ref="O30:O42" si="12">AVERAGE(B26:B29)</f>
+        <v>57.5</v>
+      </c>
+      <c r="P30" s="76">
+        <f t="shared" ref="P30:P42" si="13">AVERAGE(B26:B29)</f>
+        <v>57.5</v>
+      </c>
+      <c r="Q30" s="44">
+        <f t="shared" ref="Q30:Q41" si="14">B30-O30</f>
+        <v>33.5</v>
+      </c>
+      <c r="R30" s="66">
+        <f t="shared" ref="R30:R41" si="15">ABS(Q30)</f>
+        <v>33.5</v>
+      </c>
+      <c r="S30" s="62">
+        <f t="shared" ref="S30:S41" si="16">Q30^2</f>
+        <v>1122.25</v>
+      </c>
+      <c r="T30" s="75">
+        <f t="shared" ref="T30:T41" si="17">R30/B30</f>
+        <v>0.36813186813186816</v>
+      </c>
       <c r="V30" s="42"/>
       <c r="W30" s="42"/>
       <c r="X30" s="42"/>
@@ -4039,31 +4122,85 @@
       <c r="AI30" s="42"/>
       <c r="AJ30" s="42"/>
     </row>
-    <row r="31" spans="1:36" s="20" customFormat="1" ht="15">
+    <row r="31" spans="1:36" s="20" customFormat="1" ht="14.4">
       <c r="A31" s="20">
         <v>7</v>
       </c>
       <c r="B31" s="20">
         <v>54</v>
       </c>
-      <c r="C31" s="22"/>
-      <c r="D31" s="77"/>
-      <c r="E31" s="44"/>
-      <c r="F31" s="61"/>
-      <c r="G31" s="62"/>
-      <c r="H31" s="75"/>
-      <c r="I31" s="31"/>
-      <c r="J31" s="77"/>
-      <c r="K31" s="44"/>
-      <c r="L31" s="61"/>
-      <c r="M31" s="62"/>
-      <c r="N31" s="75"/>
-      <c r="O31" s="22"/>
-      <c r="P31" s="77"/>
-      <c r="Q31" s="44"/>
-      <c r="R31" s="66"/>
-      <c r="S31" s="62"/>
-      <c r="T31" s="75"/>
+      <c r="C31" s="22">
+        <f t="shared" si="0"/>
+        <v>80.5</v>
+      </c>
+      <c r="D31" s="76">
+        <f t="shared" si="1"/>
+        <v>80.5</v>
+      </c>
+      <c r="E31" s="44">
+        <f t="shared" si="2"/>
+        <v>-26.5</v>
+      </c>
+      <c r="F31" s="61">
+        <f t="shared" si="3"/>
+        <v>26.5</v>
+      </c>
+      <c r="G31" s="62">
+        <f t="shared" si="4"/>
+        <v>702.25</v>
+      </c>
+      <c r="H31" s="75">
+        <f t="shared" si="5"/>
+        <v>0.49074074074074076</v>
+      </c>
+      <c r="I31" s="31">
+        <f t="shared" si="6"/>
+        <v>72.333333333333329</v>
+      </c>
+      <c r="J31" s="76">
+        <f t="shared" si="7"/>
+        <v>72.333333333333329</v>
+      </c>
+      <c r="K31" s="44">
+        <f t="shared" si="8"/>
+        <v>-18.333333333333329</v>
+      </c>
+      <c r="L31" s="61">
+        <f t="shared" si="9"/>
+        <v>18.333333333333329</v>
+      </c>
+      <c r="M31" s="62">
+        <f t="shared" si="10"/>
+        <v>336.11111111111092</v>
+      </c>
+      <c r="N31" s="75">
+        <f t="shared" si="11"/>
+        <v>0.33950617283950607</v>
+      </c>
+      <c r="O31" s="22">
+        <f t="shared" si="12"/>
+        <v>69.25</v>
+      </c>
+      <c r="P31" s="76">
+        <f t="shared" si="13"/>
+        <v>69.25</v>
+      </c>
+      <c r="Q31" s="44">
+        <f t="shared" si="14"/>
+        <v>-15.25</v>
+      </c>
+      <c r="R31" s="66">
+        <f t="shared" si="15"/>
+        <v>15.25</v>
+      </c>
+      <c r="S31" s="62">
+        <f t="shared" si="16"/>
+        <v>232.5625</v>
+      </c>
+      <c r="T31" s="75">
+        <f t="shared" si="17"/>
+        <v>0.28240740740740738</v>
+      </c>
       <c r="V31" s="42"/>
       <c r="W31" s="42"/>
       <c r="X31" s="42"/>
@@ -4080,31 +4217,85 @@
       <c r="AI31" s="42"/>
       <c r="AJ31" s="42"/>
     </row>
-    <row r="32" spans="1:36" s="20" customFormat="1" ht="15">
+    <row r="32" spans="1:36" s="20" customFormat="1" ht="14.4">
       <c r="A32" s="20">
         <v>8</v>
       </c>
       <c r="B32" s="20">
         <v>60</v>
       </c>
-      <c r="C32" s="22"/>
-      <c r="D32" s="77"/>
-      <c r="E32" s="44"/>
-      <c r="F32" s="61"/>
-      <c r="G32" s="62"/>
-      <c r="H32" s="75"/>
-      <c r="I32" s="31"/>
-      <c r="J32" s="77"/>
-      <c r="K32" s="44"/>
-      <c r="L32" s="61"/>
-      <c r="M32" s="62"/>
-      <c r="N32" s="75"/>
-      <c r="O32" s="22"/>
-      <c r="P32" s="77"/>
-      <c r="Q32" s="44"/>
-      <c r="R32" s="66"/>
-      <c r="S32" s="62"/>
-      <c r="T32" s="75"/>
+      <c r="C32" s="22">
+        <f t="shared" si="0"/>
+        <v>72.5</v>
+      </c>
+      <c r="D32" s="76">
+        <f t="shared" si="1"/>
+        <v>72.5</v>
+      </c>
+      <c r="E32" s="44">
+        <f t="shared" si="2"/>
+        <v>-12.5</v>
+      </c>
+      <c r="F32" s="61">
+        <f t="shared" si="3"/>
+        <v>12.5</v>
+      </c>
+      <c r="G32" s="62">
+        <f t="shared" si="4"/>
+        <v>156.25</v>
+      </c>
+      <c r="H32" s="75">
+        <f t="shared" si="5"/>
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="I32" s="31">
+        <f t="shared" si="6"/>
+        <v>71.666666666666671</v>
+      </c>
+      <c r="J32" s="76">
+        <f t="shared" si="7"/>
+        <v>71.666666666666671</v>
+      </c>
+      <c r="K32" s="44">
+        <f t="shared" si="8"/>
+        <v>-11.666666666666671</v>
+      </c>
+      <c r="L32" s="61">
+        <f t="shared" si="9"/>
+        <v>11.666666666666671</v>
+      </c>
+      <c r="M32" s="62">
+        <f t="shared" si="10"/>
+        <v>136.11111111111123</v>
+      </c>
+      <c r="N32" s="75">
+        <f t="shared" si="11"/>
+        <v>0.19444444444444453</v>
+      </c>
+      <c r="O32" s="22">
+        <f t="shared" si="12"/>
+        <v>67.75</v>
+      </c>
+      <c r="P32" s="76">
+        <f t="shared" si="13"/>
+        <v>67.75</v>
+      </c>
+      <c r="Q32" s="44">
+        <f t="shared" si="14"/>
+        <v>-7.75</v>
+      </c>
+      <c r="R32" s="66">
+        <f t="shared" si="15"/>
+        <v>7.75</v>
+      </c>
+      <c r="S32" s="62">
+        <f t="shared" si="16"/>
+        <v>60.0625</v>
+      </c>
+      <c r="T32" s="75">
+        <f t="shared" si="17"/>
+        <v>0.12916666666666668</v>
+      </c>
       <c r="V32" s="42"/>
       <c r="W32" s="42"/>
       <c r="X32" s="42"/>
@@ -4121,31 +4312,85 @@
       <c r="AI32" s="42"/>
       <c r="AJ32" s="42"/>
     </row>
-    <row r="33" spans="1:36" s="20" customFormat="1" ht="15">
+    <row r="33" spans="1:36" s="20" customFormat="1" ht="14.4">
       <c r="A33" s="20">
         <v>9</v>
       </c>
       <c r="B33" s="20">
         <v>48</v>
       </c>
-      <c r="C33" s="22"/>
-      <c r="D33" s="77"/>
-      <c r="E33" s="44"/>
-      <c r="F33" s="61"/>
-      <c r="G33" s="62"/>
-      <c r="H33" s="75"/>
-      <c r="I33" s="31"/>
-      <c r="J33" s="77"/>
-      <c r="K33" s="44"/>
-      <c r="L33" s="61"/>
-      <c r="M33" s="62"/>
-      <c r="N33" s="75"/>
-      <c r="O33" s="22"/>
-      <c r="P33" s="77"/>
-      <c r="Q33" s="44"/>
-      <c r="R33" s="66"/>
-      <c r="S33" s="62"/>
-      <c r="T33" s="75"/>
+      <c r="C33" s="22">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="D33" s="76">
+        <f t="shared" si="1"/>
+        <v>57</v>
+      </c>
+      <c r="E33" s="44">
+        <f t="shared" si="2"/>
+        <v>-9</v>
+      </c>
+      <c r="F33" s="61">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="G33" s="62">
+        <f t="shared" si="4"/>
+        <v>81</v>
+      </c>
+      <c r="H33" s="75">
+        <f t="shared" si="5"/>
+        <v>0.1875</v>
+      </c>
+      <c r="I33" s="31">
+        <f t="shared" si="6"/>
+        <v>68.333333333333329</v>
+      </c>
+      <c r="J33" s="76">
+        <f t="shared" si="7"/>
+        <v>68.333333333333329</v>
+      </c>
+      <c r="K33" s="44">
+        <f t="shared" si="8"/>
+        <v>-20.333333333333329</v>
+      </c>
+      <c r="L33" s="61">
+        <f t="shared" si="9"/>
+        <v>20.333333333333329</v>
+      </c>
+      <c r="M33" s="62">
+        <f t="shared" si="10"/>
+        <v>413.44444444444423</v>
+      </c>
+      <c r="N33" s="75">
+        <f t="shared" si="11"/>
+        <v>0.42361111111111099</v>
+      </c>
+      <c r="O33" s="22">
+        <f t="shared" si="12"/>
+        <v>68.75</v>
+      </c>
+      <c r="P33" s="76">
+        <f t="shared" si="13"/>
+        <v>68.75</v>
+      </c>
+      <c r="Q33" s="44">
+        <f t="shared" si="14"/>
+        <v>-20.75</v>
+      </c>
+      <c r="R33" s="66">
+        <f t="shared" si="15"/>
+        <v>20.75</v>
+      </c>
+      <c r="S33" s="62">
+        <f t="shared" si="16"/>
+        <v>430.5625</v>
+      </c>
+      <c r="T33" s="75">
+        <f t="shared" si="17"/>
+        <v>0.43229166666666669</v>
+      </c>
       <c r="V33" s="42"/>
       <c r="W33" s="42"/>
       <c r="X33" s="42"/>
@@ -4162,31 +4407,85 @@
       <c r="AI33" s="42"/>
       <c r="AJ33" s="42"/>
     </row>
-    <row r="34" spans="1:36" s="20" customFormat="1" ht="15">
+    <row r="34" spans="1:36" s="20" customFormat="1" ht="14.4">
       <c r="A34" s="20">
         <v>10</v>
       </c>
       <c r="B34" s="20">
         <v>35</v>
       </c>
-      <c r="C34" s="22"/>
-      <c r="D34" s="77"/>
-      <c r="E34" s="44"/>
-      <c r="F34" s="61"/>
-      <c r="G34" s="62"/>
-      <c r="H34" s="75"/>
-      <c r="I34" s="31"/>
-      <c r="J34" s="77"/>
-      <c r="K34" s="44"/>
-      <c r="L34" s="61"/>
-      <c r="M34" s="62"/>
-      <c r="N34" s="75"/>
-      <c r="O34" s="22"/>
-      <c r="P34" s="77"/>
-      <c r="Q34" s="44"/>
-      <c r="R34" s="66"/>
-      <c r="S34" s="62"/>
-      <c r="T34" s="75"/>
+      <c r="C34" s="22">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="D34" s="76">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="E34" s="44">
+        <f t="shared" si="2"/>
+        <v>-19</v>
+      </c>
+      <c r="F34" s="61">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="G34" s="62">
+        <f t="shared" si="4"/>
+        <v>361</v>
+      </c>
+      <c r="H34" s="75">
+        <f t="shared" si="5"/>
+        <v>0.54285714285714282</v>
+      </c>
+      <c r="I34" s="31">
+        <f t="shared" si="6"/>
+        <v>54</v>
+      </c>
+      <c r="J34" s="76">
+        <f t="shared" si="7"/>
+        <v>54</v>
+      </c>
+      <c r="K34" s="44">
+        <f t="shared" si="8"/>
+        <v>-19</v>
+      </c>
+      <c r="L34" s="61">
+        <f t="shared" si="9"/>
+        <v>19</v>
+      </c>
+      <c r="M34" s="62">
+        <f t="shared" si="10"/>
+        <v>361</v>
+      </c>
+      <c r="N34" s="75">
+        <f t="shared" si="11"/>
+        <v>0.54285714285714282</v>
+      </c>
+      <c r="O34" s="22">
+        <f t="shared" si="12"/>
+        <v>63.25</v>
+      </c>
+      <c r="P34" s="76">
+        <f t="shared" si="13"/>
+        <v>63.25</v>
+      </c>
+      <c r="Q34" s="44">
+        <f t="shared" si="14"/>
+        <v>-28.25</v>
+      </c>
+      <c r="R34" s="66">
+        <f t="shared" si="15"/>
+        <v>28.25</v>
+      </c>
+      <c r="S34" s="62">
+        <f t="shared" si="16"/>
+        <v>798.0625</v>
+      </c>
+      <c r="T34" s="75">
+        <f t="shared" si="17"/>
+        <v>0.80714285714285716</v>
+      </c>
       <c r="V34" s="42"/>
       <c r="W34" s="42"/>
       <c r="X34" s="42"/>
@@ -4203,31 +4502,85 @@
       <c r="AI34" s="42"/>
       <c r="AJ34" s="42"/>
     </row>
-    <row r="35" spans="1:36" s="20" customFormat="1" ht="15">
+    <row r="35" spans="1:36" s="20" customFormat="1" ht="14.4">
       <c r="A35" s="20">
         <v>11</v>
       </c>
       <c r="B35" s="20">
         <v>49</v>
       </c>
-      <c r="C35" s="22"/>
-      <c r="D35" s="77"/>
-      <c r="E35" s="44"/>
-      <c r="F35" s="61"/>
-      <c r="G35" s="62"/>
-      <c r="H35" s="75"/>
-      <c r="I35" s="31"/>
-      <c r="J35" s="77"/>
-      <c r="K35" s="44"/>
-      <c r="L35" s="61"/>
-      <c r="M35" s="62"/>
-      <c r="N35" s="75"/>
-      <c r="O35" s="22"/>
-      <c r="P35" s="77"/>
-      <c r="Q35" s="44"/>
-      <c r="R35" s="66"/>
-      <c r="S35" s="62"/>
-      <c r="T35" s="75"/>
+      <c r="C35" s="22">
+        <f t="shared" si="0"/>
+        <v>41.5</v>
+      </c>
+      <c r="D35" s="76">
+        <f t="shared" si="1"/>
+        <v>41.5</v>
+      </c>
+      <c r="E35" s="44">
+        <f t="shared" si="2"/>
+        <v>7.5</v>
+      </c>
+      <c r="F35" s="61">
+        <f t="shared" si="3"/>
+        <v>7.5</v>
+      </c>
+      <c r="G35" s="62">
+        <f t="shared" si="4"/>
+        <v>56.25</v>
+      </c>
+      <c r="H35" s="75">
+        <f t="shared" si="5"/>
+        <v>0.15306122448979592</v>
+      </c>
+      <c r="I35" s="31">
+        <f t="shared" si="6"/>
+        <v>47.666666666666664</v>
+      </c>
+      <c r="J35" s="76">
+        <f t="shared" si="7"/>
+        <v>47.666666666666664</v>
+      </c>
+      <c r="K35" s="44">
+        <f t="shared" si="8"/>
+        <v>1.3333333333333357</v>
+      </c>
+      <c r="L35" s="61">
+        <f t="shared" si="9"/>
+        <v>1.3333333333333357</v>
+      </c>
+      <c r="M35" s="62">
+        <f t="shared" si="10"/>
+        <v>1.7777777777777841</v>
+      </c>
+      <c r="N35" s="75">
+        <f t="shared" si="11"/>
+        <v>2.7210884353741544E-2</v>
+      </c>
+      <c r="O35" s="22">
+        <f t="shared" si="12"/>
+        <v>49.25</v>
+      </c>
+      <c r="P35" s="76">
+        <f t="shared" si="13"/>
+        <v>49.25</v>
+      </c>
+      <c r="Q35" s="44">
+        <f t="shared" si="14"/>
+        <v>-0.25</v>
+      </c>
+      <c r="R35" s="66">
+        <f t="shared" si="15"/>
+        <v>0.25</v>
+      </c>
+      <c r="S35" s="62">
+        <f t="shared" si="16"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="T35" s="75">
+        <f t="shared" si="17"/>
+        <v>5.1020408163265302E-3</v>
+      </c>
       <c r="V35" s="42"/>
       <c r="W35" s="42"/>
       <c r="X35" s="42"/>
@@ -4244,31 +4597,85 @@
       <c r="AI35" s="42"/>
       <c r="AJ35" s="42"/>
     </row>
-    <row r="36" spans="1:36" s="20" customFormat="1" ht="15">
+    <row r="36" spans="1:36" s="20" customFormat="1" ht="14.4">
       <c r="A36" s="20">
         <v>12</v>
       </c>
       <c r="B36" s="20">
         <v>44</v>
       </c>
-      <c r="C36" s="22"/>
-      <c r="D36" s="77"/>
-      <c r="E36" s="44"/>
-      <c r="F36" s="61"/>
-      <c r="G36" s="62"/>
-      <c r="H36" s="75"/>
-      <c r="I36" s="31"/>
-      <c r="J36" s="77"/>
-      <c r="K36" s="44"/>
-      <c r="L36" s="61"/>
-      <c r="M36" s="62"/>
-      <c r="N36" s="75"/>
-      <c r="O36" s="22"/>
-      <c r="P36" s="77"/>
-      <c r="Q36" s="44"/>
-      <c r="R36" s="66"/>
-      <c r="S36" s="62"/>
-      <c r="T36" s="75"/>
+      <c r="C36" s="22">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="D36" s="76">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="E36" s="44">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="F36" s="61">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="G36" s="62">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="H36" s="75">
+        <f t="shared" si="5"/>
+        <v>4.5454545454545456E-2</v>
+      </c>
+      <c r="I36" s="31">
+        <f t="shared" si="6"/>
+        <v>44</v>
+      </c>
+      <c r="J36" s="76">
+        <f t="shared" si="7"/>
+        <v>44</v>
+      </c>
+      <c r="K36" s="44">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L36" s="61">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="M36" s="62">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="N36" s="75">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="O36" s="22">
+        <f t="shared" si="12"/>
+        <v>48</v>
+      </c>
+      <c r="P36" s="76">
+        <f t="shared" si="13"/>
+        <v>48</v>
+      </c>
+      <c r="Q36" s="44">
+        <f t="shared" si="14"/>
+        <v>-4</v>
+      </c>
+      <c r="R36" s="66">
+        <f t="shared" si="15"/>
+        <v>4</v>
+      </c>
+      <c r="S36" s="62">
+        <f t="shared" si="16"/>
+        <v>16</v>
+      </c>
+      <c r="T36" s="75">
+        <f t="shared" si="17"/>
+        <v>9.0909090909090912E-2</v>
+      </c>
       <c r="V36" s="42"/>
       <c r="W36" s="42"/>
       <c r="X36" s="42"/>
@@ -4285,31 +4692,85 @@
       <c r="AI36" s="42"/>
       <c r="AJ36" s="42"/>
     </row>
-    <row r="37" spans="1:36" s="20" customFormat="1" ht="15">
+    <row r="37" spans="1:36" s="20" customFormat="1" ht="14.4">
       <c r="A37" s="20">
         <v>13</v>
       </c>
       <c r="B37" s="20">
         <v>61</v>
       </c>
-      <c r="C37" s="22"/>
-      <c r="D37" s="77"/>
-      <c r="E37" s="44"/>
-      <c r="F37" s="61"/>
-      <c r="G37" s="62"/>
-      <c r="H37" s="75"/>
-      <c r="I37" s="31"/>
-      <c r="J37" s="77"/>
-      <c r="K37" s="44"/>
-      <c r="L37" s="61"/>
-      <c r="M37" s="62"/>
-      <c r="N37" s="75"/>
-      <c r="O37" s="22"/>
-      <c r="P37" s="77"/>
-      <c r="Q37" s="44"/>
-      <c r="R37" s="66"/>
-      <c r="S37" s="62"/>
-      <c r="T37" s="75"/>
+      <c r="C37" s="22">
+        <f t="shared" si="0"/>
+        <v>46.5</v>
+      </c>
+      <c r="D37" s="76">
+        <f t="shared" si="1"/>
+        <v>46.5</v>
+      </c>
+      <c r="E37" s="44">
+        <f t="shared" si="2"/>
+        <v>14.5</v>
+      </c>
+      <c r="F37" s="61">
+        <f t="shared" si="3"/>
+        <v>14.5</v>
+      </c>
+      <c r="G37" s="62">
+        <f t="shared" si="4"/>
+        <v>210.25</v>
+      </c>
+      <c r="H37" s="75">
+        <f t="shared" si="5"/>
+        <v>0.23770491803278687</v>
+      </c>
+      <c r="I37" s="31">
+        <f t="shared" si="6"/>
+        <v>42.666666666666664</v>
+      </c>
+      <c r="J37" s="76">
+        <f t="shared" si="7"/>
+        <v>42.666666666666664</v>
+      </c>
+      <c r="K37" s="44">
+        <f t="shared" si="8"/>
+        <v>18.333333333333336</v>
+      </c>
+      <c r="L37" s="61">
+        <f t="shared" si="9"/>
+        <v>18.333333333333336</v>
+      </c>
+      <c r="M37" s="62">
+        <f t="shared" si="10"/>
+        <v>336.1111111111112</v>
+      </c>
+      <c r="N37" s="75">
+        <f t="shared" si="11"/>
+        <v>0.30054644808743175</v>
+      </c>
+      <c r="O37" s="22">
+        <f t="shared" si="12"/>
+        <v>44</v>
+      </c>
+      <c r="P37" s="76">
+        <f t="shared" si="13"/>
+        <v>44</v>
+      </c>
+      <c r="Q37" s="44">
+        <f t="shared" si="14"/>
+        <v>17</v>
+      </c>
+      <c r="R37" s="66">
+        <f t="shared" si="15"/>
+        <v>17</v>
+      </c>
+      <c r="S37" s="62">
+        <f t="shared" si="16"/>
+        <v>289</v>
+      </c>
+      <c r="T37" s="75">
+        <f t="shared" si="17"/>
+        <v>0.27868852459016391</v>
+      </c>
       <c r="V37" s="42"/>
       <c r="W37" s="42"/>
       <c r="X37" s="42"/>
@@ -4326,31 +4787,85 @@
       <c r="AI37" s="42"/>
       <c r="AJ37" s="42"/>
     </row>
-    <row r="38" spans="1:36" s="20" customFormat="1" ht="15">
+    <row r="38" spans="1:36" s="20" customFormat="1" ht="14.4">
       <c r="A38" s="20">
         <v>14</v>
       </c>
       <c r="B38" s="20">
         <v>68</v>
       </c>
-      <c r="C38" s="22"/>
-      <c r="D38" s="77"/>
-      <c r="E38" s="44"/>
-      <c r="F38" s="61"/>
-      <c r="G38" s="62"/>
-      <c r="H38" s="75"/>
-      <c r="I38" s="31"/>
-      <c r="J38" s="77"/>
-      <c r="K38" s="44"/>
-      <c r="L38" s="61"/>
-      <c r="M38" s="62"/>
-      <c r="N38" s="75"/>
-      <c r="O38" s="22"/>
-      <c r="P38" s="77"/>
-      <c r="Q38" s="44"/>
-      <c r="R38" s="66"/>
-      <c r="S38" s="62"/>
-      <c r="T38" s="75"/>
+      <c r="C38" s="22">
+        <f t="shared" si="0"/>
+        <v>52.5</v>
+      </c>
+      <c r="D38" s="76">
+        <f t="shared" si="1"/>
+        <v>52.5</v>
+      </c>
+      <c r="E38" s="44">
+        <f t="shared" si="2"/>
+        <v>15.5</v>
+      </c>
+      <c r="F38" s="61">
+        <f t="shared" si="3"/>
+        <v>15.5</v>
+      </c>
+      <c r="G38" s="62">
+        <f t="shared" si="4"/>
+        <v>240.25</v>
+      </c>
+      <c r="H38" s="75">
+        <f t="shared" si="5"/>
+        <v>0.22794117647058823</v>
+      </c>
+      <c r="I38" s="31">
+        <f t="shared" si="6"/>
+        <v>51.333333333333336</v>
+      </c>
+      <c r="J38" s="76">
+        <f t="shared" si="7"/>
+        <v>51.333333333333336</v>
+      </c>
+      <c r="K38" s="44">
+        <f t="shared" si="8"/>
+        <v>16.666666666666664</v>
+      </c>
+      <c r="L38" s="61">
+        <f t="shared" si="9"/>
+        <v>16.666666666666664</v>
+      </c>
+      <c r="M38" s="62">
+        <f t="shared" si="10"/>
+        <v>277.77777777777771</v>
+      </c>
+      <c r="N38" s="75">
+        <f t="shared" si="11"/>
+        <v>0.24509803921568624</v>
+      </c>
+      <c r="O38" s="22">
+        <f t="shared" si="12"/>
+        <v>47.25</v>
+      </c>
+      <c r="P38" s="76">
+        <f t="shared" si="13"/>
+        <v>47.25</v>
+      </c>
+      <c r="Q38" s="44">
+        <f t="shared" si="14"/>
+        <v>20.75</v>
+      </c>
+      <c r="R38" s="66">
+        <f t="shared" si="15"/>
+        <v>20.75</v>
+      </c>
+      <c r="S38" s="62">
+        <f t="shared" si="16"/>
+        <v>430.5625</v>
+      </c>
+      <c r="T38" s="75">
+        <f t="shared" si="17"/>
+        <v>0.30514705882352944</v>
+      </c>
       <c r="V38" s="42"/>
       <c r="W38" s="42"/>
       <c r="X38" s="42"/>
@@ -4367,31 +4882,85 @@
       <c r="AI38" s="42"/>
       <c r="AJ38" s="42"/>
     </row>
-    <row r="39" spans="1:36" s="20" customFormat="1" ht="15">
+    <row r="39" spans="1:36" s="20" customFormat="1" ht="14.4">
       <c r="A39" s="20">
         <v>15</v>
       </c>
       <c r="B39" s="20">
         <v>82</v>
       </c>
-      <c r="C39" s="22"/>
-      <c r="D39" s="77"/>
-      <c r="E39" s="44"/>
-      <c r="F39" s="61"/>
-      <c r="G39" s="62"/>
-      <c r="H39" s="75"/>
-      <c r="I39" s="31"/>
-      <c r="J39" s="77"/>
-      <c r="K39" s="44"/>
-      <c r="L39" s="61"/>
-      <c r="M39" s="62"/>
-      <c r="N39" s="75"/>
-      <c r="O39" s="22"/>
-      <c r="P39" s="77"/>
-      <c r="Q39" s="44"/>
-      <c r="R39" s="66"/>
-      <c r="S39" s="62"/>
-      <c r="T39" s="75"/>
+      <c r="C39" s="22">
+        <f t="shared" si="0"/>
+        <v>64.5</v>
+      </c>
+      <c r="D39" s="76">
+        <f t="shared" si="1"/>
+        <v>64.5</v>
+      </c>
+      <c r="E39" s="44">
+        <f t="shared" si="2"/>
+        <v>17.5</v>
+      </c>
+      <c r="F39" s="61">
+        <f t="shared" si="3"/>
+        <v>17.5</v>
+      </c>
+      <c r="G39" s="62">
+        <f t="shared" si="4"/>
+        <v>306.25</v>
+      </c>
+      <c r="H39" s="75">
+        <f t="shared" si="5"/>
+        <v>0.21341463414634146</v>
+      </c>
+      <c r="I39" s="31">
+        <f t="shared" si="6"/>
+        <v>57.666666666666664</v>
+      </c>
+      <c r="J39" s="76">
+        <f t="shared" si="7"/>
+        <v>57.666666666666664</v>
+      </c>
+      <c r="K39" s="44">
+        <f t="shared" si="8"/>
+        <v>24.333333333333336</v>
+      </c>
+      <c r="L39" s="61">
+        <f t="shared" si="9"/>
+        <v>24.333333333333336</v>
+      </c>
+      <c r="M39" s="62">
+        <f t="shared" si="10"/>
+        <v>592.1111111111112</v>
+      </c>
+      <c r="N39" s="75">
+        <f t="shared" si="11"/>
+        <v>0.2967479674796748</v>
+      </c>
+      <c r="O39" s="22">
+        <f t="shared" si="12"/>
+        <v>55.5</v>
+      </c>
+      <c r="P39" s="76">
+        <f t="shared" si="13"/>
+        <v>55.5</v>
+      </c>
+      <c r="Q39" s="44">
+        <f t="shared" si="14"/>
+        <v>26.5</v>
+      </c>
+      <c r="R39" s="66">
+        <f t="shared" si="15"/>
+        <v>26.5</v>
+      </c>
+      <c r="S39" s="62">
+        <f t="shared" si="16"/>
+        <v>702.25</v>
+      </c>
+      <c r="T39" s="75">
+        <f t="shared" si="17"/>
+        <v>0.32317073170731708</v>
+      </c>
       <c r="V39" s="42"/>
       <c r="W39" s="42"/>
       <c r="X39" s="42"/>
@@ -4408,31 +4977,85 @@
       <c r="AI39" s="42"/>
       <c r="AJ39" s="42"/>
     </row>
-    <row r="40" spans="1:36" s="20" customFormat="1" ht="15">
+    <row r="40" spans="1:36" s="20" customFormat="1" ht="14.4">
       <c r="A40" s="20">
         <v>16</v>
       </c>
       <c r="B40" s="20">
         <v>71</v>
       </c>
-      <c r="C40" s="22"/>
-      <c r="D40" s="77"/>
-      <c r="E40" s="44"/>
-      <c r="F40" s="61"/>
-      <c r="G40" s="62"/>
-      <c r="H40" s="75"/>
-      <c r="I40" s="31"/>
-      <c r="J40" s="77"/>
-      <c r="K40" s="44"/>
-      <c r="L40" s="61"/>
-      <c r="M40" s="62"/>
-      <c r="N40" s="75"/>
-      <c r="O40" s="22"/>
-      <c r="P40" s="77"/>
-      <c r="Q40" s="44"/>
-      <c r="R40" s="66"/>
-      <c r="S40" s="62"/>
-      <c r="T40" s="75"/>
+      <c r="C40" s="22">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="D40" s="76">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="E40" s="44">
+        <f t="shared" si="2"/>
+        <v>-4</v>
+      </c>
+      <c r="F40" s="61">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="G40" s="62">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="H40" s="75">
+        <f t="shared" si="5"/>
+        <v>5.6338028169014086E-2</v>
+      </c>
+      <c r="I40" s="31">
+        <f t="shared" si="6"/>
+        <v>70.333333333333329</v>
+      </c>
+      <c r="J40" s="76">
+        <f t="shared" si="7"/>
+        <v>70.333333333333329</v>
+      </c>
+      <c r="K40" s="44">
+        <f t="shared" si="8"/>
+        <v>0.6666666666666714</v>
+      </c>
+      <c r="L40" s="61">
+        <f t="shared" si="9"/>
+        <v>0.6666666666666714</v>
+      </c>
+      <c r="M40" s="62">
+        <f t="shared" si="10"/>
+        <v>0.44444444444445075</v>
+      </c>
+      <c r="N40" s="75">
+        <f t="shared" si="11"/>
+        <v>9.3896713615024135E-3</v>
+      </c>
+      <c r="O40" s="22">
+        <f t="shared" si="12"/>
+        <v>63.75</v>
+      </c>
+      <c r="P40" s="76">
+        <f t="shared" si="13"/>
+        <v>63.75</v>
+      </c>
+      <c r="Q40" s="44">
+        <f t="shared" si="14"/>
+        <v>7.25</v>
+      </c>
+      <c r="R40" s="66">
+        <f t="shared" si="15"/>
+        <v>7.25</v>
+      </c>
+      <c r="S40" s="62">
+        <f t="shared" si="16"/>
+        <v>52.5625</v>
+      </c>
+      <c r="T40" s="75">
+        <f t="shared" si="17"/>
+        <v>0.10211267605633803</v>
+      </c>
       <c r="V40" s="42"/>
       <c r="W40" s="42"/>
       <c r="X40" s="42"/>
@@ -4449,31 +5072,85 @@
       <c r="AI40" s="42"/>
       <c r="AJ40" s="42"/>
     </row>
-    <row r="41" spans="1:36" s="20" customFormat="1" ht="16" thickBot="1">
+    <row r="41" spans="1:36" s="20" customFormat="1" ht="15" thickBot="1">
       <c r="A41" s="20">
         <v>17</v>
       </c>
       <c r="B41" s="20">
         <v>50</v>
       </c>
-      <c r="C41" s="76"/>
-      <c r="D41" s="77"/>
-      <c r="E41" s="44"/>
-      <c r="F41" s="61"/>
-      <c r="G41" s="62"/>
-      <c r="H41" s="75"/>
-      <c r="I41" s="76"/>
-      <c r="J41" s="78"/>
-      <c r="K41" s="44"/>
-      <c r="L41" s="61"/>
-      <c r="M41" s="62"/>
-      <c r="N41" s="75"/>
-      <c r="O41" s="76"/>
-      <c r="P41" s="78"/>
-      <c r="Q41" s="44"/>
-      <c r="R41" s="66"/>
-      <c r="S41" s="62"/>
-      <c r="T41" s="75"/>
+      <c r="C41" s="22">
+        <f t="shared" si="0"/>
+        <v>76.5</v>
+      </c>
+      <c r="D41" s="76">
+        <f t="shared" si="1"/>
+        <v>76.5</v>
+      </c>
+      <c r="E41" s="44">
+        <f t="shared" si="2"/>
+        <v>-26.5</v>
+      </c>
+      <c r="F41" s="61">
+        <f t="shared" si="3"/>
+        <v>26.5</v>
+      </c>
+      <c r="G41" s="62">
+        <f t="shared" si="4"/>
+        <v>702.25</v>
+      </c>
+      <c r="H41" s="75">
+        <f t="shared" si="5"/>
+        <v>0.53</v>
+      </c>
+      <c r="I41" s="31">
+        <f t="shared" si="6"/>
+        <v>73.666666666666671</v>
+      </c>
+      <c r="J41" s="76">
+        <f t="shared" si="7"/>
+        <v>73.666666666666671</v>
+      </c>
+      <c r="K41" s="44">
+        <f t="shared" si="8"/>
+        <v>-23.666666666666671</v>
+      </c>
+      <c r="L41" s="61">
+        <f t="shared" si="9"/>
+        <v>23.666666666666671</v>
+      </c>
+      <c r="M41" s="62">
+        <f t="shared" si="10"/>
+        <v>560.11111111111131</v>
+      </c>
+      <c r="N41" s="75">
+        <f t="shared" si="11"/>
+        <v>0.47333333333333344</v>
+      </c>
+      <c r="O41" s="22">
+        <f t="shared" si="12"/>
+        <v>70.5</v>
+      </c>
+      <c r="P41" s="76">
+        <f t="shared" si="13"/>
+        <v>70.5</v>
+      </c>
+      <c r="Q41" s="44">
+        <f t="shared" si="14"/>
+        <v>-20.5</v>
+      </c>
+      <c r="R41" s="66">
+        <f t="shared" si="15"/>
+        <v>20.5</v>
+      </c>
+      <c r="S41" s="62">
+        <f t="shared" si="16"/>
+        <v>420.25</v>
+      </c>
+      <c r="T41" s="75">
+        <f t="shared" si="17"/>
+        <v>0.41</v>
+      </c>
       <c r="V41" s="42"/>
       <c r="W41" s="42"/>
       <c r="X41" s="42"/>
@@ -4490,31 +5167,76 @@
       <c r="AI41" s="42"/>
       <c r="AJ41" s="42"/>
     </row>
-    <row r="42" spans="1:36" s="20" customFormat="1" ht="16" thickBot="1">
+    <row r="42" spans="1:36" s="20" customFormat="1" ht="15" thickBot="1">
       <c r="A42" s="23">
         <v>18</v>
       </c>
       <c r="B42" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="C42" s="22"/>
-      <c r="D42" s="109"/>
-      <c r="E42" s="45"/>
-      <c r="F42" s="81"/>
-      <c r="G42" s="82"/>
-      <c r="H42" s="83"/>
-      <c r="I42" s="31"/>
-      <c r="J42" s="77"/>
+      <c r="C42" s="22">
+        <f>AVERAGE(B40:B41)</f>
+        <v>60.5</v>
+      </c>
+      <c r="D42" s="76">
+        <f t="shared" si="1"/>
+        <v>60.5</v>
+      </c>
+      <c r="E42" s="44"/>
+      <c r="F42" s="78">
+        <f>AVERAGE(F27:F41)</f>
+        <v>13.633333333333333</v>
+      </c>
+      <c r="G42" s="79">
+        <f>AVERAGE(G27:G41)</f>
+        <v>254.38333333333333</v>
+      </c>
+      <c r="H42" s="80">
+        <f>AVERAGE(H27:H41)</f>
+        <v>0.2362596796162493</v>
+      </c>
+      <c r="I42" s="31">
+        <f>AVERAGE(B39:B41)</f>
+        <v>67.666666666666671</v>
+      </c>
+      <c r="J42" s="76">
+        <f t="shared" si="7"/>
+        <v>67.666666666666671</v>
+      </c>
       <c r="K42" s="46"/>
-      <c r="L42" s="81"/>
-      <c r="M42" s="82"/>
-      <c r="N42" s="83"/>
-      <c r="O42" s="22"/>
-      <c r="P42" s="77"/>
+      <c r="L42" s="78">
+        <f>AVERAGE(L28:L41)</f>
+        <v>14.857142857142861</v>
+      </c>
+      <c r="M42" s="79">
+        <f>AVERAGE(M28:M41)</f>
+        <v>299.84126984126988</v>
+      </c>
+      <c r="N42" s="80">
+        <f>AVERAGE(N28:N41)</f>
+        <v>0.25374135105123391</v>
+      </c>
+      <c r="O42" s="22">
+        <f t="shared" si="12"/>
+        <v>67.75</v>
+      </c>
+      <c r="P42" s="76">
+        <f t="shared" si="13"/>
+        <v>67.75</v>
+      </c>
       <c r="Q42" s="45"/>
-      <c r="R42" s="84"/>
-      <c r="S42" s="82"/>
-      <c r="T42" s="83"/>
+      <c r="R42" s="81">
+        <f>AVERAGE(R29:R41)</f>
+        <v>16.134615384615383</v>
+      </c>
+      <c r="S42" s="79">
+        <f>AVERAGE(S29:S41)</f>
+        <v>355.24519230769232</v>
+      </c>
+      <c r="T42" s="80">
+        <f>AVERAGE(T29:T41)</f>
+        <v>0.28065817716953434</v>
+      </c>
       <c r="V42" s="42"/>
       <c r="W42" s="42"/>
       <c r="X42" s="42"/>
@@ -4532,10 +5254,10 @@
       <c r="AJ42" s="42"/>
     </row>
     <row r="43" spans="1:36" ht="15.75" customHeight="1" thickBot="1">
-      <c r="C43" s="92" t="s">
+      <c r="C43" s="83" t="s">
         <v>16</v>
       </c>
-      <c r="D43" s="93"/>
+      <c r="D43" s="84"/>
       <c r="E43" s="35"/>
       <c r="F43" s="32" t="s">
         <v>6</v>
@@ -4543,13 +5265,13 @@
       <c r="G43" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="H43" s="108" t="s">
+      <c r="H43" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="94" t="s">
+      <c r="I43" s="85" t="s">
         <v>16</v>
       </c>
-      <c r="J43" s="94"/>
+      <c r="J43" s="85"/>
       <c r="K43" s="34"/>
       <c r="L43" s="25" t="s">
         <v>6</v>
@@ -4560,10 +5282,10 @@
       <c r="N43" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="O43" s="95" t="s">
+      <c r="O43" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="P43" s="96"/>
+      <c r="P43" s="87"/>
       <c r="Q43" s="24"/>
       <c r="R43" s="38" t="s">
         <v>6</v>
@@ -4626,7 +5348,7 @@
       <c r="AI45" s="9"/>
       <c r="AJ45" s="9"/>
     </row>
-    <row r="46" spans="1:36" ht="14" thickBot="1">
+    <row r="46" spans="1:36" ht="13.8" thickBot="1">
       <c r="P46" s="2"/>
     </row>
     <row r="47" spans="1:36">
@@ -4659,23 +5381,23 @@
       <c r="AE47" s="9"/>
       <c r="AF47" s="9"/>
     </row>
-    <row r="48" spans="1:36" ht="15">
-      <c r="C48" s="87" t="s">
+    <row r="48" spans="1:36" ht="14.4">
+      <c r="C48" s="89" t="s">
         <v>20</v>
       </c>
-      <c r="D48" s="88"/>
-      <c r="E48" s="87" t="s">
+      <c r="D48" s="90"/>
+      <c r="E48" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="F48" s="88"/>
-      <c r="G48" s="87" t="s">
+      <c r="F48" s="90"/>
+      <c r="G48" s="89" t="s">
         <v>22</v>
       </c>
-      <c r="H48" s="88"/>
-      <c r="I48" s="87" t="s">
+      <c r="H48" s="90"/>
+      <c r="I48" s="89" t="s">
         <v>23</v>
       </c>
-      <c r="J48" s="88"/>
+      <c r="J48" s="90"/>
       <c r="K48"/>
       <c r="L48"/>
       <c r="M48"/>
@@ -4695,7 +5417,7 @@
       <c r="AE48" s="9"/>
       <c r="AF48" s="9"/>
     </row>
-    <row r="49" spans="1:32" ht="43" thickBot="1">
+    <row r="49" spans="1:32" ht="40.200000000000003" thickBot="1">
       <c r="A49" s="17" t="s">
         <v>0</v>
       </c>
@@ -4745,20 +5467,32 @@
       <c r="AE49" s="9"/>
       <c r="AF49" s="9"/>
     </row>
-    <row r="50" spans="1:32" s="20" customFormat="1" ht="14" thickTop="1">
+    <row r="50" spans="1:32" s="20" customFormat="1" ht="13.8" thickTop="1">
       <c r="A50" s="20">
         <v>1</v>
       </c>
       <c r="B50" s="50">
         <v>88</v>
       </c>
-      <c r="C50" s="51"/>
+      <c r="C50" s="51">
+        <f>B50</f>
+        <v>88</v>
+      </c>
       <c r="D50"/>
-      <c r="E50" s="51"/>
+      <c r="E50" s="51">
+        <f>B50</f>
+        <v>88</v>
+      </c>
       <c r="F50"/>
-      <c r="G50" s="21"/>
+      <c r="G50" s="21">
+        <f>B50</f>
+        <v>88</v>
+      </c>
       <c r="H50"/>
-      <c r="I50" s="21"/>
+      <c r="I50" s="21">
+        <f>B50</f>
+        <v>88</v>
+      </c>
       <c r="J50"/>
       <c r="K50" s="54"/>
       <c r="L50"/>
@@ -4784,14 +5518,38 @@
       <c r="B51" s="20">
         <v>44</v>
       </c>
-      <c r="C51" s="51"/>
-      <c r="D51" s="77"/>
-      <c r="E51" s="51"/>
-      <c r="F51"/>
-      <c r="G51" s="22"/>
-      <c r="H51" s="77"/>
-      <c r="I51" s="22"/>
-      <c r="J51" s="77"/>
+      <c r="C51" s="51">
+        <f>0.4*B50+(1-0.4)*C50</f>
+        <v>88</v>
+      </c>
+      <c r="D51" s="76">
+        <f>C51</f>
+        <v>88</v>
+      </c>
+      <c r="E51" s="51">
+        <f>0.5*B50+(1-0.5)*E50</f>
+        <v>88</v>
+      </c>
+      <c r="F51" s="76">
+        <f>E51</f>
+        <v>88</v>
+      </c>
+      <c r="G51" s="22">
+        <f>0.6*B50+(1-0.6)*G50</f>
+        <v>88</v>
+      </c>
+      <c r="H51" s="76">
+        <f>G51</f>
+        <v>88</v>
+      </c>
+      <c r="I51" s="22">
+        <f>0.7*B50+(1-0.7)*I50</f>
+        <v>88</v>
+      </c>
+      <c r="J51" s="76">
+        <f>I51</f>
+        <v>88</v>
+      </c>
       <c r="K51" s="54"/>
       <c r="L51"/>
       <c r="M51"/>
@@ -4816,14 +5574,38 @@
       <c r="B52" s="20">
         <v>60</v>
       </c>
-      <c r="C52" s="51"/>
-      <c r="D52" s="77"/>
-      <c r="E52" s="51"/>
-      <c r="F52"/>
-      <c r="G52" s="22"/>
-      <c r="H52" s="77"/>
-      <c r="I52" s="22"/>
-      <c r="J52" s="77"/>
+      <c r="C52" s="51">
+        <f t="shared" ref="C52:C67" si="18">0.4*B51+(1-0.4)*C51</f>
+        <v>70.400000000000006</v>
+      </c>
+      <c r="D52" s="76">
+        <f t="shared" ref="D52:D66" si="19">C52</f>
+        <v>70.400000000000006</v>
+      </c>
+      <c r="E52" s="51">
+        <f t="shared" ref="E52:E67" si="20">0.5*B51+(1-0.5)*E51</f>
+        <v>66</v>
+      </c>
+      <c r="F52" s="76">
+        <f t="shared" ref="F52:F66" si="21">E52</f>
+        <v>66</v>
+      </c>
+      <c r="G52" s="22">
+        <f t="shared" ref="G52:G67" si="22">0.6*B51+(1-0.6)*G51</f>
+        <v>61.6</v>
+      </c>
+      <c r="H52" s="76">
+        <f t="shared" ref="H52:H66" si="23">G52</f>
+        <v>61.6</v>
+      </c>
+      <c r="I52" s="22">
+        <f t="shared" ref="I52:I67" si="24">0.7*B51+(1-0.7)*I51</f>
+        <v>57.2</v>
+      </c>
+      <c r="J52" s="76">
+        <f t="shared" ref="J52:J66" si="25">I52</f>
+        <v>57.2</v>
+      </c>
       <c r="K52" s="54"/>
       <c r="L52"/>
       <c r="M52"/>
@@ -4848,14 +5630,38 @@
       <c r="B53" s="20">
         <v>56</v>
       </c>
-      <c r="C53" s="51"/>
-      <c r="D53" s="77"/>
-      <c r="E53" s="51"/>
-      <c r="F53"/>
-      <c r="G53" s="22"/>
-      <c r="H53" s="77"/>
-      <c r="I53" s="22"/>
-      <c r="J53" s="77"/>
+      <c r="C53" s="51">
+        <f t="shared" si="18"/>
+        <v>66.240000000000009</v>
+      </c>
+      <c r="D53" s="76">
+        <f t="shared" si="19"/>
+        <v>66.240000000000009</v>
+      </c>
+      <c r="E53" s="51">
+        <f t="shared" si="20"/>
+        <v>63</v>
+      </c>
+      <c r="F53" s="76">
+        <f t="shared" si="21"/>
+        <v>63</v>
+      </c>
+      <c r="G53" s="22">
+        <f t="shared" si="22"/>
+        <v>60.64</v>
+      </c>
+      <c r="H53" s="76">
+        <f t="shared" si="23"/>
+        <v>60.64</v>
+      </c>
+      <c r="I53" s="22">
+        <f t="shared" si="24"/>
+        <v>59.160000000000004</v>
+      </c>
+      <c r="J53" s="76">
+        <f t="shared" si="25"/>
+        <v>59.160000000000004</v>
+      </c>
       <c r="K53" s="54"/>
       <c r="L53"/>
       <c r="M53"/>
@@ -4880,14 +5686,38 @@
       <c r="B54" s="20">
         <v>70</v>
       </c>
-      <c r="C54" s="51"/>
-      <c r="D54" s="77"/>
-      <c r="E54" s="51"/>
-      <c r="F54"/>
-      <c r="G54" s="22"/>
-      <c r="H54" s="77"/>
-      <c r="I54" s="22"/>
-      <c r="J54" s="77"/>
+      <c r="C54" s="51">
+        <f t="shared" si="18"/>
+        <v>62.144000000000005</v>
+      </c>
+      <c r="D54" s="76">
+        <f t="shared" si="19"/>
+        <v>62.144000000000005</v>
+      </c>
+      <c r="E54" s="51">
+        <f t="shared" si="20"/>
+        <v>59.5</v>
+      </c>
+      <c r="F54" s="76">
+        <f t="shared" si="21"/>
+        <v>59.5</v>
+      </c>
+      <c r="G54" s="22">
+        <f t="shared" si="22"/>
+        <v>57.856000000000002</v>
+      </c>
+      <c r="H54" s="76">
+        <f t="shared" si="23"/>
+        <v>57.856000000000002</v>
+      </c>
+      <c r="I54" s="22">
+        <f t="shared" si="24"/>
+        <v>56.948</v>
+      </c>
+      <c r="J54" s="76">
+        <f t="shared" si="25"/>
+        <v>56.948</v>
+      </c>
       <c r="K54" s="54"/>
       <c r="L54"/>
       <c r="M54"/>
@@ -4912,14 +5742,38 @@
       <c r="B55" s="20">
         <v>91</v>
       </c>
-      <c r="C55" s="51"/>
-      <c r="D55" s="77"/>
-      <c r="E55" s="51"/>
-      <c r="F55"/>
-      <c r="G55" s="22"/>
-      <c r="H55" s="77"/>
-      <c r="I55" s="22"/>
-      <c r="J55" s="77"/>
+      <c r="C55" s="51">
+        <f t="shared" si="18"/>
+        <v>65.2864</v>
+      </c>
+      <c r="D55" s="76">
+        <f t="shared" si="19"/>
+        <v>65.2864</v>
+      </c>
+      <c r="E55" s="51">
+        <f t="shared" si="20"/>
+        <v>64.75</v>
+      </c>
+      <c r="F55" s="76">
+        <f t="shared" si="21"/>
+        <v>64.75</v>
+      </c>
+      <c r="G55" s="22">
+        <f t="shared" si="22"/>
+        <v>65.142400000000009</v>
+      </c>
+      <c r="H55" s="76">
+        <f t="shared" si="23"/>
+        <v>65.142400000000009</v>
+      </c>
+      <c r="I55" s="22">
+        <f t="shared" si="24"/>
+        <v>66.084400000000002</v>
+      </c>
+      <c r="J55" s="76">
+        <f t="shared" si="25"/>
+        <v>66.084400000000002</v>
+      </c>
       <c r="K55" s="54"/>
       <c r="L55"/>
       <c r="M55"/>
@@ -4944,14 +5798,38 @@
       <c r="B56" s="20">
         <v>54</v>
       </c>
-      <c r="C56" s="51"/>
-      <c r="D56" s="77"/>
-      <c r="E56" s="51"/>
-      <c r="F56"/>
-      <c r="G56" s="22"/>
-      <c r="H56" s="77"/>
-      <c r="I56" s="22"/>
-      <c r="J56" s="77"/>
+      <c r="C56" s="51">
+        <f t="shared" si="18"/>
+        <v>75.571839999999995</v>
+      </c>
+      <c r="D56" s="76">
+        <f t="shared" si="19"/>
+        <v>75.571839999999995</v>
+      </c>
+      <c r="E56" s="51">
+        <f t="shared" si="20"/>
+        <v>77.875</v>
+      </c>
+      <c r="F56" s="76">
+        <f t="shared" si="21"/>
+        <v>77.875</v>
+      </c>
+      <c r="G56" s="22">
+        <f t="shared" si="22"/>
+        <v>80.656959999999998</v>
+      </c>
+      <c r="H56" s="76">
+        <f t="shared" si="23"/>
+        <v>80.656959999999998</v>
+      </c>
+      <c r="I56" s="22">
+        <f t="shared" si="24"/>
+        <v>83.525319999999994</v>
+      </c>
+      <c r="J56" s="76">
+        <f t="shared" si="25"/>
+        <v>83.525319999999994</v>
+      </c>
       <c r="K56" s="54"/>
       <c r="L56"/>
       <c r="M56"/>
@@ -4976,14 +5854,38 @@
       <c r="B57" s="20">
         <v>60</v>
       </c>
-      <c r="C57" s="51"/>
-      <c r="D57" s="77"/>
-      <c r="E57" s="51"/>
-      <c r="F57"/>
-      <c r="G57" s="22"/>
-      <c r="H57" s="77"/>
-      <c r="I57" s="22"/>
-      <c r="J57" s="77"/>
+      <c r="C57" s="51">
+        <f t="shared" si="18"/>
+        <v>66.943104000000005</v>
+      </c>
+      <c r="D57" s="76">
+        <f t="shared" si="19"/>
+        <v>66.943104000000005</v>
+      </c>
+      <c r="E57" s="51">
+        <f t="shared" si="20"/>
+        <v>65.9375</v>
+      </c>
+      <c r="F57" s="76">
+        <f t="shared" si="21"/>
+        <v>65.9375</v>
+      </c>
+      <c r="G57" s="22">
+        <f t="shared" si="22"/>
+        <v>64.662784000000002</v>
+      </c>
+      <c r="H57" s="76">
+        <f t="shared" si="23"/>
+        <v>64.662784000000002</v>
+      </c>
+      <c r="I57" s="22">
+        <f t="shared" si="24"/>
+        <v>62.857596000000001</v>
+      </c>
+      <c r="J57" s="76">
+        <f t="shared" si="25"/>
+        <v>62.857596000000001</v>
+      </c>
       <c r="K57" s="54"/>
       <c r="L57"/>
       <c r="M57"/>
@@ -5008,14 +5910,38 @@
       <c r="B58" s="20">
         <v>48</v>
       </c>
-      <c r="C58" s="51"/>
-      <c r="D58" s="77"/>
-      <c r="E58" s="51"/>
-      <c r="F58"/>
-      <c r="G58" s="22"/>
-      <c r="H58" s="77"/>
-      <c r="I58" s="22"/>
-      <c r="J58" s="77"/>
+      <c r="C58" s="51">
+        <f t="shared" si="18"/>
+        <v>64.165862400000009</v>
+      </c>
+      <c r="D58" s="76">
+        <f t="shared" si="19"/>
+        <v>64.165862400000009</v>
+      </c>
+      <c r="E58" s="51">
+        <f t="shared" si="20"/>
+        <v>62.96875</v>
+      </c>
+      <c r="F58" s="76">
+        <f t="shared" si="21"/>
+        <v>62.96875</v>
+      </c>
+      <c r="G58" s="22">
+        <f t="shared" si="22"/>
+        <v>61.865113600000001</v>
+      </c>
+      <c r="H58" s="76">
+        <f t="shared" si="23"/>
+        <v>61.865113600000001</v>
+      </c>
+      <c r="I58" s="22">
+        <f t="shared" si="24"/>
+        <v>60.857278800000003</v>
+      </c>
+      <c r="J58" s="76">
+        <f t="shared" si="25"/>
+        <v>60.857278800000003</v>
+      </c>
       <c r="K58" s="54"/>
       <c r="L58"/>
       <c r="M58"/>
@@ -5040,14 +5966,38 @@
       <c r="B59" s="20">
         <v>35</v>
       </c>
-      <c r="C59" s="51"/>
-      <c r="D59" s="77"/>
-      <c r="E59" s="51"/>
-      <c r="F59"/>
-      <c r="G59" s="22"/>
-      <c r="H59" s="77"/>
-      <c r="I59" s="22"/>
-      <c r="J59" s="77"/>
+      <c r="C59" s="51">
+        <f t="shared" si="18"/>
+        <v>57.699517440000008</v>
+      </c>
+      <c r="D59" s="76">
+        <f t="shared" si="19"/>
+        <v>57.699517440000008</v>
+      </c>
+      <c r="E59" s="51">
+        <f t="shared" si="20"/>
+        <v>55.484375</v>
+      </c>
+      <c r="F59" s="76">
+        <f t="shared" si="21"/>
+        <v>55.484375</v>
+      </c>
+      <c r="G59" s="22">
+        <f t="shared" si="22"/>
+        <v>53.54604544</v>
+      </c>
+      <c r="H59" s="76">
+        <f t="shared" si="23"/>
+        <v>53.54604544</v>
+      </c>
+      <c r="I59" s="22">
+        <f t="shared" si="24"/>
+        <v>51.857183640000002</v>
+      </c>
+      <c r="J59" s="76">
+        <f t="shared" si="25"/>
+        <v>51.857183640000002</v>
+      </c>
       <c r="K59" s="54"/>
       <c r="L59"/>
       <c r="M59"/>
@@ -5072,14 +6022,38 @@
       <c r="B60" s="20">
         <v>49</v>
       </c>
-      <c r="C60" s="51"/>
-      <c r="D60" s="77"/>
-      <c r="E60" s="51"/>
-      <c r="F60"/>
-      <c r="G60" s="22"/>
-      <c r="H60" s="77"/>
-      <c r="I60" s="22"/>
-      <c r="J60" s="77"/>
+      <c r="C60" s="51">
+        <f t="shared" si="18"/>
+        <v>48.619710464000001</v>
+      </c>
+      <c r="D60" s="76">
+        <f t="shared" si="19"/>
+        <v>48.619710464000001</v>
+      </c>
+      <c r="E60" s="51">
+        <f t="shared" si="20"/>
+        <v>45.2421875</v>
+      </c>
+      <c r="F60" s="76">
+        <f t="shared" si="21"/>
+        <v>45.2421875</v>
+      </c>
+      <c r="G60" s="22">
+        <f t="shared" si="22"/>
+        <v>42.418418176000003</v>
+      </c>
+      <c r="H60" s="76">
+        <f t="shared" si="23"/>
+        <v>42.418418176000003</v>
+      </c>
+      <c r="I60" s="22">
+        <f t="shared" si="24"/>
+        <v>40.057155092000002</v>
+      </c>
+      <c r="J60" s="76">
+        <f t="shared" si="25"/>
+        <v>40.057155092000002</v>
+      </c>
       <c r="K60" s="54"/>
       <c r="L60"/>
       <c r="M60"/>
@@ -5104,14 +6078,38 @@
       <c r="B61" s="20">
         <v>44</v>
       </c>
-      <c r="C61" s="51"/>
-      <c r="D61" s="77"/>
-      <c r="E61" s="51"/>
-      <c r="F61"/>
-      <c r="G61" s="22"/>
-      <c r="H61" s="77"/>
-      <c r="I61" s="22"/>
-      <c r="J61" s="77"/>
+      <c r="C61" s="51">
+        <f t="shared" si="18"/>
+        <v>48.771826278399999</v>
+      </c>
+      <c r="D61" s="76">
+        <f t="shared" si="19"/>
+        <v>48.771826278399999</v>
+      </c>
+      <c r="E61" s="51">
+        <f t="shared" si="20"/>
+        <v>47.12109375</v>
+      </c>
+      <c r="F61" s="76">
+        <f t="shared" si="21"/>
+        <v>47.12109375</v>
+      </c>
+      <c r="G61" s="22">
+        <f t="shared" si="22"/>
+        <v>46.367367270399996</v>
+      </c>
+      <c r="H61" s="76">
+        <f t="shared" si="23"/>
+        <v>46.367367270399996</v>
+      </c>
+      <c r="I61" s="22">
+        <f t="shared" si="24"/>
+        <v>46.317146527600002</v>
+      </c>
+      <c r="J61" s="76">
+        <f t="shared" si="25"/>
+        <v>46.317146527600002</v>
+      </c>
       <c r="K61" s="54"/>
       <c r="L61"/>
       <c r="M61"/>
@@ -5136,14 +6134,38 @@
       <c r="B62" s="20">
         <v>61</v>
       </c>
-      <c r="C62" s="51"/>
-      <c r="D62" s="77"/>
-      <c r="E62" s="51"/>
-      <c r="F62"/>
-      <c r="G62" s="22"/>
-      <c r="H62" s="77"/>
-      <c r="I62" s="22"/>
-      <c r="J62" s="77"/>
+      <c r="C62" s="51">
+        <f t="shared" si="18"/>
+        <v>46.863095767040001</v>
+      </c>
+      <c r="D62" s="76">
+        <f t="shared" si="19"/>
+        <v>46.863095767040001</v>
+      </c>
+      <c r="E62" s="51">
+        <f t="shared" si="20"/>
+        <v>45.560546875</v>
+      </c>
+      <c r="F62" s="76">
+        <f t="shared" si="21"/>
+        <v>45.560546875</v>
+      </c>
+      <c r="G62" s="22">
+        <f t="shared" si="22"/>
+        <v>44.946946908160001</v>
+      </c>
+      <c r="H62" s="76">
+        <f t="shared" si="23"/>
+        <v>44.946946908160001</v>
+      </c>
+      <c r="I62" s="22">
+        <f t="shared" si="24"/>
+        <v>44.695143958279999</v>
+      </c>
+      <c r="J62" s="76">
+        <f t="shared" si="25"/>
+        <v>44.695143958279999</v>
+      </c>
       <c r="K62" s="54"/>
       <c r="L62"/>
       <c r="M62"/>
@@ -5168,14 +6190,38 @@
       <c r="B63" s="20">
         <v>68</v>
       </c>
-      <c r="C63" s="51"/>
-      <c r="D63" s="77"/>
-      <c r="E63" s="51"/>
-      <c r="F63"/>
-      <c r="G63" s="22"/>
-      <c r="H63" s="77"/>
-      <c r="I63" s="22"/>
-      <c r="J63" s="77"/>
+      <c r="C63" s="51">
+        <f t="shared" si="18"/>
+        <v>52.517857460224</v>
+      </c>
+      <c r="D63" s="76">
+        <f t="shared" si="19"/>
+        <v>52.517857460224</v>
+      </c>
+      <c r="E63" s="51">
+        <f t="shared" si="20"/>
+        <v>53.2802734375</v>
+      </c>
+      <c r="F63" s="76">
+        <f t="shared" si="21"/>
+        <v>53.2802734375</v>
+      </c>
+      <c r="G63" s="22">
+        <f t="shared" si="22"/>
+        <v>54.578778763263998</v>
+      </c>
+      <c r="H63" s="76">
+        <f t="shared" si="23"/>
+        <v>54.578778763263998</v>
+      </c>
+      <c r="I63" s="22">
+        <f t="shared" si="24"/>
+        <v>56.108543187483995</v>
+      </c>
+      <c r="J63" s="76">
+        <f t="shared" si="25"/>
+        <v>56.108543187483995</v>
+      </c>
       <c r="K63" s="54"/>
       <c r="L63"/>
       <c r="M63"/>
@@ -5200,14 +6246,38 @@
       <c r="B64" s="20">
         <v>82</v>
       </c>
-      <c r="C64" s="51"/>
-      <c r="D64" s="77"/>
-      <c r="E64" s="51"/>
-      <c r="F64"/>
-      <c r="G64" s="22"/>
-      <c r="H64" s="77"/>
-      <c r="I64" s="22"/>
-      <c r="J64" s="77"/>
+      <c r="C64" s="51">
+        <f t="shared" si="18"/>
+        <v>58.710714476134399</v>
+      </c>
+      <c r="D64" s="76">
+        <f t="shared" si="19"/>
+        <v>58.710714476134399</v>
+      </c>
+      <c r="E64" s="51">
+        <f t="shared" si="20"/>
+        <v>60.64013671875</v>
+      </c>
+      <c r="F64" s="76">
+        <f t="shared" si="21"/>
+        <v>60.64013671875</v>
+      </c>
+      <c r="G64" s="22">
+        <f t="shared" si="22"/>
+        <v>62.631511505305596</v>
+      </c>
+      <c r="H64" s="76">
+        <f t="shared" si="23"/>
+        <v>62.631511505305596</v>
+      </c>
+      <c r="I64" s="22">
+        <f t="shared" si="24"/>
+        <v>64.432562956245192</v>
+      </c>
+      <c r="J64" s="76">
+        <f t="shared" si="25"/>
+        <v>64.432562956245192</v>
+      </c>
       <c r="K64" s="54"/>
       <c r="L64"/>
       <c r="M64"/>
@@ -5231,14 +6301,38 @@
       <c r="B65" s="20">
         <v>71</v>
       </c>
-      <c r="C65" s="51"/>
-      <c r="D65" s="77"/>
-      <c r="E65" s="51"/>
-      <c r="F65"/>
-      <c r="G65" s="22"/>
-      <c r="H65" s="77"/>
-      <c r="I65" s="22"/>
-      <c r="J65" s="77"/>
+      <c r="C65" s="51">
+        <f t="shared" si="18"/>
+        <v>68.026428685680642</v>
+      </c>
+      <c r="D65" s="76">
+        <f t="shared" si="19"/>
+        <v>68.026428685680642</v>
+      </c>
+      <c r="E65" s="51">
+        <f t="shared" si="20"/>
+        <v>71.320068359375</v>
+      </c>
+      <c r="F65" s="76">
+        <f t="shared" si="21"/>
+        <v>71.320068359375</v>
+      </c>
+      <c r="G65" s="22">
+        <f t="shared" si="22"/>
+        <v>74.252604602122233</v>
+      </c>
+      <c r="H65" s="76">
+        <f t="shared" si="23"/>
+        <v>74.252604602122233</v>
+      </c>
+      <c r="I65" s="22">
+        <f t="shared" si="24"/>
+        <v>76.729768886873558</v>
+      </c>
+      <c r="J65" s="76">
+        <f t="shared" si="25"/>
+        <v>76.729768886873558</v>
+      </c>
       <c r="K65" s="54"/>
       <c r="L65"/>
       <c r="M65"/>
@@ -5254,21 +6348,45 @@
       <c r="W65" s="42"/>
       <c r="X65" s="42"/>
     </row>
-    <row r="66" spans="1:29" s="20" customFormat="1" ht="14" thickBot="1">
+    <row r="66" spans="1:29" s="20" customFormat="1" ht="13.8" thickBot="1">
       <c r="A66" s="20">
         <v>17</v>
       </c>
       <c r="B66" s="20">
         <v>50</v>
       </c>
-      <c r="C66" s="51"/>
-      <c r="D66" s="107"/>
-      <c r="E66" s="79"/>
-      <c r="F66"/>
-      <c r="G66" s="76"/>
-      <c r="H66" s="77"/>
-      <c r="I66" s="76"/>
-      <c r="J66" s="77"/>
+      <c r="C66" s="51">
+        <f t="shared" si="18"/>
+        <v>69.215857211408391</v>
+      </c>
+      <c r="D66" s="76">
+        <f t="shared" si="19"/>
+        <v>69.215857211408391</v>
+      </c>
+      <c r="E66" s="51">
+        <f t="shared" si="20"/>
+        <v>71.1600341796875</v>
+      </c>
+      <c r="F66" s="76">
+        <f t="shared" si="21"/>
+        <v>71.1600341796875</v>
+      </c>
+      <c r="G66" s="22">
+        <f t="shared" si="22"/>
+        <v>72.301041840848896</v>
+      </c>
+      <c r="H66" s="76">
+        <f t="shared" si="23"/>
+        <v>72.301041840848896</v>
+      </c>
+      <c r="I66" s="22">
+        <f t="shared" si="24"/>
+        <v>72.718930666062064</v>
+      </c>
+      <c r="J66" s="76">
+        <f t="shared" si="25"/>
+        <v>72.718930666062064</v>
+      </c>
       <c r="K66" s="54"/>
       <c r="L66"/>
       <c r="M66"/>
@@ -5284,20 +6402,32 @@
       <c r="W66" s="42"/>
       <c r="X66" s="42"/>
     </row>
-    <row r="67" spans="1:29" s="20" customFormat="1" ht="14" thickBot="1">
+    <row r="67" spans="1:29" s="20" customFormat="1" ht="13.8" thickBot="1">
       <c r="A67" s="23">
         <v>18</v>
       </c>
       <c r="B67" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C67" s="110"/>
-      <c r="D67" s="77"/>
-      <c r="E67" s="51"/>
-      <c r="F67" s="80"/>
-      <c r="G67" s="22"/>
+      <c r="C67" s="51">
+        <f t="shared" si="18"/>
+        <v>61.529514326845032</v>
+      </c>
+      <c r="D67" s="76"/>
+      <c r="E67" s="51">
+        <f t="shared" si="20"/>
+        <v>60.58001708984375</v>
+      </c>
+      <c r="F67" s="77"/>
+      <c r="G67" s="22">
+        <f t="shared" si="22"/>
+        <v>58.920416736339561</v>
+      </c>
       <c r="H67" s="55"/>
-      <c r="I67" s="22"/>
+      <c r="I67" s="22">
+        <f t="shared" si="24"/>
+        <v>56.815679199818618</v>
+      </c>
       <c r="J67" s="56"/>
       <c r="K67"/>
       <c r="L67"/>
@@ -5314,24 +6444,24 @@
       <c r="W67" s="42"/>
       <c r="X67" s="42"/>
     </row>
-    <row r="68" spans="1:29" ht="14" thickBot="1">
+    <row r="68" spans="1:29" ht="13.8" thickBot="1">
       <c r="B68" s="9"/>
-      <c r="C68" s="102" t="s">
+      <c r="C68" s="91" t="s">
         <v>16</v>
       </c>
-      <c r="D68" s="103"/>
-      <c r="E68" s="104" t="s">
+      <c r="D68" s="92"/>
+      <c r="E68" s="93" t="s">
         <v>16</v>
       </c>
-      <c r="F68" s="105"/>
-      <c r="G68" s="104" t="s">
+      <c r="F68" s="94"/>
+      <c r="G68" s="93" t="s">
         <v>16</v>
       </c>
-      <c r="H68" s="105"/>
-      <c r="I68" s="104" t="s">
+      <c r="H68" s="94"/>
+      <c r="I68" s="93" t="s">
         <v>16</v>
       </c>
-      <c r="J68" s="106"/>
+      <c r="J68" s="95"/>
       <c r="K68"/>
       <c r="L68"/>
       <c r="M68"/>
@@ -5349,17 +6479,29 @@
       <c r="Y68" s="3"/>
       <c r="AC68" s="3"/>
     </row>
-    <row r="69" spans="1:29" ht="15">
+    <row r="69" spans="1:29" ht="14.4">
       <c r="A69" s="9"/>
       <c r="B69" s="9"/>
-      <c r="C69" s="97"/>
-      <c r="D69" s="98"/>
-      <c r="E69" s="99"/>
-      <c r="F69" s="100"/>
-      <c r="G69" s="99"/>
-      <c r="H69" s="100"/>
-      <c r="I69" s="99"/>
-      <c r="J69" s="101"/>
+      <c r="C69" s="101">
+        <f>SUMXMY2(B51:B66,D51:D66)/COUNT(D51:D66)</f>
+        <v>346.56397464149831</v>
+      </c>
+      <c r="D69" s="88"/>
+      <c r="E69" s="101">
+        <f>SUMXMY2(B51:B66,F51:F66)/COUNT(F51:F66)</f>
+        <v>340.76611377764493</v>
+      </c>
+      <c r="F69" s="88"/>
+      <c r="G69" s="101">
+        <f>SUMXMY2(B51:B66,H51:H66)/COUNT(H51:H66)</f>
+        <v>338.40747825272939</v>
+      </c>
+      <c r="H69" s="88"/>
+      <c r="I69" s="101">
+        <f>SUMXMY2(B51:B66,J51:J66)/COUNT(J51:J66)</f>
+        <v>339.03410543199334</v>
+      </c>
+      <c r="J69" s="88"/>
       <c r="K69"/>
       <c r="L69"/>
       <c r="M69"/>
@@ -5376,24 +6518,24 @@
       <c r="X69" s="9"/>
       <c r="AC69" s="3"/>
     </row>
-    <row r="70" spans="1:29" ht="16" thickBot="1">
+    <row r="70" spans="1:29" ht="15" thickBot="1">
       <c r="B70" s="9"/>
-      <c r="C70" s="89" t="s">
+      <c r="C70" s="98" t="s">
         <v>7</v>
       </c>
-      <c r="D70" s="90"/>
-      <c r="E70" s="85" t="s">
+      <c r="D70" s="99"/>
+      <c r="E70" s="96" t="s">
         <v>7</v>
       </c>
-      <c r="F70" s="91"/>
-      <c r="G70" s="85" t="s">
+      <c r="F70" s="100"/>
+      <c r="G70" s="96" t="s">
         <v>7</v>
       </c>
-      <c r="H70" s="91"/>
-      <c r="I70" s="85" t="s">
+      <c r="H70" s="100"/>
+      <c r="I70" s="96" t="s">
         <v>7</v>
       </c>
-      <c r="J70" s="86"/>
+      <c r="J70" s="97"/>
       <c r="K70"/>
       <c r="L70"/>
       <c r="M70"/>
@@ -5428,6 +6570,12 @@
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="19">
+    <mergeCell ref="I70:J70"/>
+    <mergeCell ref="I48:J48"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="E70:F70"/>
+    <mergeCell ref="G70:H70"/>
     <mergeCell ref="C43:D43"/>
     <mergeCell ref="I43:J43"/>
     <mergeCell ref="O43:P43"/>
@@ -5441,12 +6589,6 @@
     <mergeCell ref="E68:F68"/>
     <mergeCell ref="G68:H68"/>
     <mergeCell ref="I68:J68"/>
-    <mergeCell ref="I70:J70"/>
-    <mergeCell ref="I48:J48"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="E70:F70"/>
-    <mergeCell ref="G70:H70"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>